<commit_message>
data and dashboard edits
</commit_message>
<xml_diff>
--- a/data/claim_percentage.xlsx
+++ b/data/claim_percentage.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayeg\OneDrive\Desktop\Job Applications\Clipboard Health\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayeg\OneDrive\Desktop\Job Applications\Clipboard Health\CBH_dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A0E681-E693-411D-BFD6-03F71CB50454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADD87C0-1531-430C-B0FE-3A6D34F668DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -411,10 +411,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E125"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="11.9296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.53125" bestFit="1" customWidth="1"/>
@@ -440,801 +443,801 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>16.666666666666661</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5">
-        <v>3.773584905660377</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E6">
-        <v>6.5217391304347823</v>
+        <v>46.428571428571431</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
-        <v>551</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>0.72595281306715065</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>440</v>
+        <v>13</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E8">
-        <v>1.5909090909090911</v>
+        <v>38.461538461538467</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>305</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>4.5901639344262293</v>
+        <v>33.333333333333329</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10">
-        <v>847</v>
+        <v>16</v>
       </c>
       <c r="D10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E10">
-        <v>1.1806375442739081</v>
+        <v>31.25</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>2967</v>
+        <v>42</v>
       </c>
       <c r="D11">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="E11">
-        <v>1.7526120660599931</v>
+        <v>28.571428571428569</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12">
-        <v>1965</v>
+        <v>14</v>
       </c>
       <c r="D12">
-        <v>74</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>3.7659033078880402</v>
+        <v>28.571428571428569</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13">
-        <v>3854</v>
+        <v>58</v>
       </c>
       <c r="D13">
-        <v>104</v>
+        <v>16</v>
       </c>
       <c r="E13">
-        <v>2.698495070057084</v>
+        <v>27.586206896551719</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C14">
-        <v>5985</v>
+        <v>115</v>
       </c>
       <c r="D14">
-        <v>107</v>
+        <v>24</v>
       </c>
       <c r="E14">
-        <v>1.7878028404344199</v>
+        <v>20.869565217391301</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15">
-        <v>4019</v>
+        <v>456</v>
       </c>
       <c r="D15">
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="E15">
-        <v>3.4834535954217469</v>
+        <v>20.614035087719301</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16">
-        <v>7560</v>
+        <v>335</v>
       </c>
       <c r="D16">
-        <v>153</v>
+        <v>69</v>
       </c>
       <c r="E16">
-        <v>2.0238095238095242</v>
+        <v>20.597014925373131</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C17">
-        <v>11804</v>
+        <v>526</v>
       </c>
       <c r="D17">
-        <v>290</v>
+        <v>107</v>
       </c>
       <c r="E17">
-        <v>2.456794307014571</v>
+        <v>20.342205323193919</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18">
-        <v>6765</v>
+        <v>20</v>
       </c>
       <c r="D18">
-        <v>262</v>
+        <v>4</v>
       </c>
       <c r="E18">
-        <v>3.8728750923872872</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19">
-        <v>14229</v>
+        <v>92</v>
       </c>
       <c r="D19">
-        <v>308</v>
+        <v>18</v>
       </c>
       <c r="E19">
-        <v>2.1645934359406849</v>
+        <v>19.565217391304351</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C20">
-        <v>23192</v>
+        <v>751</v>
       </c>
       <c r="D20">
-        <v>843</v>
+        <v>142</v>
       </c>
       <c r="E20">
-        <v>3.6348740945153502</v>
+        <v>18.90812250332889</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
       </c>
       <c r="C21">
-        <v>14997</v>
+        <v>334</v>
       </c>
       <c r="D21">
-        <v>642</v>
+        <v>61</v>
       </c>
       <c r="E21">
-        <v>4.2808561712342472</v>
+        <v>18.26347305389222</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22">
-        <v>32596</v>
-      </c>
       <c r="D22">
-        <v>1118</v>
+        <v>4</v>
       </c>
       <c r="E22">
-        <v>3.429868695545466</v>
+        <v>18.18181818181818</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23">
-        <v>12442</v>
+        <v>39</v>
       </c>
       <c r="D23">
-        <v>590</v>
+        <v>7</v>
       </c>
       <c r="E23">
-        <v>4.7420028934254939</v>
+        <v>17.948717948717949</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
       </c>
       <c r="C24">
-        <v>7113</v>
+        <v>28</v>
       </c>
       <c r="D24">
-        <v>424</v>
+        <v>5</v>
       </c>
       <c r="E24">
-        <v>5.960916631519753</v>
+        <v>17.857142857142861</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C25">
-        <v>15846</v>
+        <v>6</v>
       </c>
       <c r="D25">
-        <v>593</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>3.7422693424208</v>
+        <v>16.666666666666661</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26">
-        <v>8504</v>
+        <v>131</v>
       </c>
       <c r="D26">
-        <v>382</v>
+        <v>21</v>
       </c>
       <c r="E26">
-        <v>4.4920037629350897</v>
+        <v>16.03053435114504</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C27">
-        <v>3783</v>
+        <v>26</v>
       </c>
       <c r="D27">
-        <v>309</v>
+        <v>4</v>
       </c>
       <c r="E27">
-        <v>8.1681205392545593</v>
+        <v>15.38461538461539</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
       <c r="C28">
-        <v>9382</v>
+        <v>13</v>
       </c>
       <c r="D28">
-        <v>536</v>
+        <v>2</v>
       </c>
       <c r="E28">
-        <v>5.7130675762097631</v>
+        <v>15.38461538461539</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C29">
-        <v>6386</v>
+        <v>550</v>
       </c>
       <c r="D29">
-        <v>270</v>
+        <v>81</v>
       </c>
       <c r="E29">
-        <v>4.2279987472596314</v>
+        <v>14.72727272727273</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C30">
-        <v>3281</v>
+        <v>256</v>
       </c>
       <c r="D30">
-        <v>225</v>
+        <v>37</v>
       </c>
       <c r="E30">
-        <v>6.8576653459311192</v>
+        <v>14.453125</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31">
-        <v>6821</v>
+        <v>555</v>
       </c>
       <c r="D31">
-        <v>351</v>
+        <v>80</v>
       </c>
       <c r="E31">
-        <v>5.1458730391438214</v>
+        <v>14.414414414414409</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C32">
-        <v>4542</v>
+        <v>21</v>
       </c>
       <c r="D32">
-        <v>225</v>
+        <v>3</v>
       </c>
       <c r="E32">
-        <v>4.9537648612945837</v>
+        <v>14.285714285714279</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33">
-        <v>2050</v>
+        <v>43</v>
       </c>
       <c r="D33">
-        <v>139</v>
+        <v>6</v>
       </c>
       <c r="E33">
-        <v>6.7804878048780486</v>
+        <v>13.95348837209302</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C34">
-        <v>4809</v>
+        <v>36</v>
       </c>
       <c r="D34">
-        <v>259</v>
+        <v>5</v>
       </c>
       <c r="E34">
-        <v>5.3857350800582244</v>
+        <v>13.888888888888889</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C35">
-        <v>3381</v>
+        <v>95</v>
       </c>
       <c r="D35">
-        <v>191</v>
+        <v>13</v>
       </c>
       <c r="E35">
-        <v>5.6492162082224189</v>
+        <v>13.684210526315789</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C36">
-        <v>1499</v>
+        <v>118</v>
       </c>
       <c r="D36">
-        <v>115</v>
+        <v>16</v>
       </c>
       <c r="E36">
-        <v>7.671781187458306</v>
+        <v>13.559322033898299</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
         <v>7</v>
       </c>
       <c r="C37">
-        <v>2968</v>
+        <v>746</v>
       </c>
       <c r="D37">
-        <v>209</v>
+        <v>101</v>
       </c>
       <c r="E37">
-        <v>7.0417789757412406</v>
+        <v>13.53887399463807</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
         <v>5</v>
       </c>
       <c r="C38">
-        <v>2406</v>
+        <v>791</v>
       </c>
       <c r="D38">
-        <v>141</v>
+        <v>104</v>
       </c>
       <c r="E38">
-        <v>5.8603491271820447</v>
+        <v>13.14791403286978</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39">
-        <v>1382</v>
+        <v>767</v>
       </c>
       <c r="D39">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="E39">
-        <v>6.0781476121562958</v>
+        <v>12.90743155149935</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C40">
-        <v>1998</v>
+        <v>449</v>
       </c>
       <c r="D40">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="E40">
-        <v>7.1571571571571564</v>
+        <v>12.694877505567931</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C41">
-        <v>1620</v>
+        <v>363</v>
       </c>
       <c r="D41">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="E41">
-        <v>5.1851851851851851</v>
+        <v>12.672176308539949</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C42">
-        <v>1143</v>
+        <v>676</v>
       </c>
       <c r="D42">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="E42">
-        <v>5.5993000874890644</v>
+        <v>12.278106508875741</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C43">
-        <v>1652</v>
+        <v>148</v>
       </c>
       <c r="D43">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="E43">
-        <v>6.3559322033898296</v>
+        <v>12.16216216216216</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C44">
-        <v>1109</v>
+        <v>149</v>
       </c>
       <c r="D44">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="E44">
-        <v>8.0252479711451752</v>
+        <v>12.080536912751681</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45">
-        <v>778</v>
+        <v>767</v>
       </c>
       <c r="D45">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="E45">
-        <v>9.5115681233933156</v>
+        <v>11.864406779661021</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B46" t="s">
         <v>7</v>
       </c>
       <c r="C46">
-        <v>1193</v>
+        <v>539</v>
       </c>
       <c r="D46">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="E46">
-        <v>7.7116512992455988</v>
+        <v>11.688311688311691</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B47" t="s">
         <v>5</v>
       </c>
       <c r="C47">
-        <v>1334</v>
+        <v>241</v>
       </c>
       <c r="D47">
-        <v>139</v>
+        <v>28</v>
       </c>
       <c r="E47">
-        <v>10.419790104947531</v>
+        <v>11.61825726141079</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C48">
-        <v>660</v>
+        <v>218</v>
       </c>
       <c r="D48">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="E48">
-        <v>11.36363636363636</v>
+        <v>11.467889908256881</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.45">
@@ -1242,50 +1245,50 @@
         <v>31</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C49">
-        <v>1293</v>
+        <v>660</v>
       </c>
       <c r="D49">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="E49">
-        <v>9.435421500386699</v>
+        <v>11.36363636363636</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C50">
-        <v>2245</v>
+        <v>18</v>
       </c>
       <c r="D50">
-        <v>232</v>
+        <v>2</v>
       </c>
       <c r="E50">
-        <v>10.334075723830731</v>
+        <v>11.111111111111111</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C51">
-        <v>659</v>
+        <v>1334</v>
       </c>
       <c r="D51">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="E51">
-        <v>10.166919575113811</v>
+        <v>10.419790104947531</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
@@ -1293,1098 +1296,1098 @@
         <v>32</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C52">
-        <v>2082</v>
+        <v>2245</v>
       </c>
       <c r="D52">
-        <v>204</v>
+        <v>232</v>
       </c>
       <c r="E52">
-        <v>9.7982708933717575</v>
+        <v>10.334075723830731</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C53">
-        <v>1936</v>
+        <v>659</v>
       </c>
       <c r="D53">
-        <v>193</v>
+        <v>67</v>
       </c>
       <c r="E53">
-        <v>9.9690082644628095</v>
+        <v>10.166919575113811</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B54" t="s">
         <v>6</v>
       </c>
       <c r="C54">
-        <v>550</v>
+        <v>227</v>
       </c>
       <c r="D54">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="E54">
-        <v>14.72727272727273</v>
+        <v>10.13215859030837</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C55">
-        <v>1522</v>
+        <v>1232</v>
       </c>
       <c r="D55">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="E55">
-        <v>9.2641261498028911</v>
+        <v>10.064935064935071</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B56" t="s">
         <v>5</v>
       </c>
       <c r="C56">
-        <v>1232</v>
+        <v>1936</v>
       </c>
       <c r="D56">
-        <v>124</v>
+        <v>193</v>
       </c>
       <c r="E56">
-        <v>10.064935064935071</v>
+        <v>9.9690082644628095</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C57">
-        <v>449</v>
+        <v>2082</v>
       </c>
       <c r="D57">
-        <v>57</v>
+        <v>204</v>
       </c>
       <c r="E57">
-        <v>12.694877505567931</v>
+        <v>9.7982708933717575</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
       </c>
       <c r="C58">
-        <v>676</v>
+        <v>126</v>
       </c>
       <c r="D58">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="E58">
-        <v>12.278106508875741</v>
+        <v>9.5238095238095237</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C59">
-        <v>791</v>
+        <v>778</v>
       </c>
       <c r="D59">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="E59">
-        <v>13.14791403286978</v>
+        <v>9.5115681233933156</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C60">
-        <v>334</v>
+        <v>1293</v>
       </c>
       <c r="D60">
-        <v>61</v>
+        <v>122</v>
       </c>
       <c r="E60">
-        <v>18.26347305389222</v>
+        <v>9.435421500386699</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B61" t="s">
         <v>7</v>
       </c>
       <c r="C61">
-        <v>456</v>
+        <v>1522</v>
       </c>
       <c r="D61">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="E61">
-        <v>20.614035087719301</v>
+        <v>9.2641261498028911</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C62">
-        <v>767</v>
+        <v>114</v>
       </c>
       <c r="D62">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="E62">
-        <v>12.90743155149935</v>
+        <v>8.7719298245614024</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C63">
-        <v>335</v>
+        <v>857</v>
       </c>
       <c r="D63">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E63">
-        <v>20.597014925373131</v>
+        <v>8.7514585764294051</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C64">
-        <v>526</v>
+        <v>351</v>
       </c>
       <c r="D64">
-        <v>107</v>
+        <v>30</v>
       </c>
       <c r="E64">
-        <v>20.342205323193919</v>
+        <v>8.5470085470085468</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B65" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C65">
-        <v>767</v>
+        <v>3783</v>
       </c>
       <c r="D65">
-        <v>91</v>
+        <v>309</v>
       </c>
       <c r="E65">
-        <v>11.864406779661021</v>
+        <v>8.1681205392545593</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B66" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C66">
-        <v>555</v>
+        <v>1109</v>
       </c>
       <c r="D66">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E66">
-        <v>14.414414414414409</v>
+        <v>8.0252479711451752</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B67" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C67">
-        <v>751</v>
+        <v>76</v>
       </c>
       <c r="D67">
-        <v>142</v>
+        <v>6</v>
       </c>
       <c r="E67">
-        <v>18.90812250332889</v>
+        <v>7.8947368421052628</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C68">
-        <v>857</v>
+        <v>1193</v>
       </c>
       <c r="D68">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="E68">
-        <v>8.7514585764294051</v>
+        <v>7.7116512992455988</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B69" t="s">
         <v>6</v>
       </c>
       <c r="C69">
-        <v>725</v>
+        <v>1499</v>
       </c>
       <c r="D69">
-        <v>54</v>
+        <v>115</v>
       </c>
       <c r="E69">
-        <v>7.4482758620689644</v>
+        <v>7.671781187458306</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B70" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C70">
-        <v>746</v>
+        <v>446</v>
       </c>
       <c r="D70">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="E70">
-        <v>13.53887399463807</v>
+        <v>7.623318385650224</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C71">
-        <v>663</v>
+        <v>66</v>
       </c>
       <c r="D71">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="E71">
-        <v>5.7315233785822022</v>
+        <v>7.5757575757575761</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B72" t="s">
         <v>6</v>
       </c>
       <c r="C72">
-        <v>537</v>
+        <v>725</v>
       </c>
       <c r="D72">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="E72">
-        <v>5.9590316573556796</v>
+        <v>7.4482758620689644</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B73" t="s">
         <v>7</v>
       </c>
       <c r="C73">
-        <v>539</v>
+        <v>1998</v>
       </c>
       <c r="D73">
-        <v>63</v>
+        <v>143</v>
       </c>
       <c r="E73">
-        <v>11.688311688311691</v>
+        <v>7.1571571571571564</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C74">
-        <v>446</v>
+        <v>2968</v>
       </c>
       <c r="D74">
-        <v>34</v>
+        <v>209</v>
       </c>
       <c r="E74">
-        <v>7.623318385650224</v>
+        <v>7.0417789757412406</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B75" t="s">
         <v>6</v>
       </c>
       <c r="C75">
-        <v>351</v>
+        <v>3281</v>
       </c>
       <c r="D75">
-        <v>30</v>
+        <v>225</v>
       </c>
       <c r="E75">
-        <v>8.5470085470085468</v>
+        <v>6.8576653459311192</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B76" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C76">
-        <v>363</v>
+        <v>2050</v>
       </c>
       <c r="D76">
-        <v>46</v>
+        <v>139</v>
       </c>
       <c r="E76">
-        <v>12.672176308539949</v>
+        <v>6.7804878048780486</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B77" t="s">
         <v>5</v>
       </c>
       <c r="C77">
-        <v>241</v>
+        <v>210</v>
       </c>
       <c r="D77">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E77">
-        <v>11.61825726141079</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="B78" t="s">
         <v>6</v>
       </c>
       <c r="C78">
-        <v>227</v>
+        <v>46</v>
       </c>
       <c r="D78">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E78">
-        <v>10.13215859030837</v>
+        <v>6.5217391304347823</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B79" t="s">
         <v>7</v>
       </c>
       <c r="C79">
-        <v>256</v>
+        <v>1652</v>
       </c>
       <c r="D79">
-        <v>37</v>
+        <v>105</v>
       </c>
       <c r="E79">
-        <v>14.453125</v>
+        <v>6.3559322033898296</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A80">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C80">
-        <v>218</v>
+        <v>1382</v>
       </c>
       <c r="D80">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="E80">
-        <v>11.467889908256881</v>
+        <v>6.0781476121562958</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A81">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B81" t="s">
         <v>6</v>
       </c>
       <c r="C81">
-        <v>148</v>
+        <v>7113</v>
       </c>
       <c r="D81">
-        <v>18</v>
+        <v>424</v>
       </c>
       <c r="E81">
-        <v>12.16216216216216</v>
+        <v>5.960916631519753</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A82">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B82" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C82">
-        <v>149</v>
+        <v>537</v>
       </c>
       <c r="D82">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E82">
-        <v>12.080536912751681</v>
+        <v>5.9590316573556796</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A83">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B83" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C83">
-        <v>210</v>
+        <v>17</v>
       </c>
       <c r="D83">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E83">
-        <v>6.666666666666667</v>
+        <v>5.8823529411764701</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A84">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B84" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C84">
-        <v>92</v>
+        <v>2406</v>
       </c>
       <c r="D84">
-        <v>18</v>
+        <v>141</v>
       </c>
       <c r="E84">
-        <v>19.565217391304351</v>
+        <v>5.8603491271820447</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A85">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B85" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C85">
-        <v>115</v>
+        <v>663</v>
       </c>
       <c r="D85">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="E85">
-        <v>20.869565217391301</v>
+        <v>5.7315233785822022</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A86">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B86" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C86">
-        <v>131</v>
+        <v>9382</v>
       </c>
       <c r="D86">
-        <v>21</v>
+        <v>536</v>
       </c>
       <c r="E86">
-        <v>16.03053435114504</v>
+        <v>5.7130675762097631</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A87">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B87" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C87">
-        <v>95</v>
+        <v>3381</v>
       </c>
       <c r="D87">
-        <v>13</v>
+        <v>191</v>
       </c>
       <c r="E87">
-        <v>13.684210526315789</v>
+        <v>5.6492162082224189</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A88">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B88" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C88">
-        <v>58</v>
+        <v>1143</v>
       </c>
       <c r="D88">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="E88">
-        <v>27.586206896551719</v>
+        <v>5.5993000874890644</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A89">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="B89" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C89">
-        <v>76</v>
+        <v>4809</v>
       </c>
       <c r="D89">
-        <v>6</v>
+        <v>259</v>
       </c>
       <c r="E89">
-        <v>7.8947368421052628</v>
+        <v>5.3857350800582244</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A90">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B90" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C90">
-        <v>66</v>
+        <v>1620</v>
       </c>
       <c r="D90">
-        <v>5</v>
+        <v>84</v>
       </c>
       <c r="E90">
-        <v>7.5757575757575761</v>
+        <v>5.1851851851851851</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A91">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="B91" t="s">
         <v>7</v>
       </c>
       <c r="C91">
-        <v>28</v>
+        <v>6821</v>
       </c>
       <c r="D91">
-        <v>13</v>
+        <v>351</v>
       </c>
       <c r="E91">
-        <v>46.428571428571431</v>
+        <v>5.1458730391438214</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A92">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="B92" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C92">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D92">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E92">
-        <v>17.948717948717949</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A93">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B93" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C93">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="D93">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E93">
-        <v>28.571428571428569</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A94">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="B94" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C94">
-        <v>114</v>
+        <v>4542</v>
       </c>
       <c r="D94">
-        <v>10</v>
+        <v>225</v>
       </c>
       <c r="E94">
-        <v>8.7719298245614024</v>
+        <v>4.9537648612945837</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A95">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B95" t="s">
         <v>5</v>
       </c>
       <c r="C95">
-        <v>43</v>
+        <v>12442</v>
       </c>
       <c r="D95">
-        <v>6</v>
+        <v>590</v>
       </c>
       <c r="E95">
-        <v>13.95348837209302</v>
+        <v>4.7420028934254939</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A96">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="B96" t="s">
         <v>6</v>
       </c>
       <c r="C96">
-        <v>22</v>
+        <v>305</v>
       </c>
       <c r="D96">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E96">
-        <v>18.18181818181818</v>
+        <v>4.5901639344262293</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A97">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B97" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C97">
-        <v>126</v>
+        <v>8504</v>
       </c>
       <c r="D97">
-        <v>12</v>
+        <v>382</v>
       </c>
       <c r="E97">
-        <v>9.5238095238095237</v>
+        <v>4.4920037629350897</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A98">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="B98" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C98">
-        <v>36</v>
+        <v>14997</v>
       </c>
       <c r="D98">
-        <v>5</v>
+        <v>642</v>
       </c>
       <c r="E98">
-        <v>13.888888888888889</v>
+        <v>4.2808561712342472</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A99">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B99" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C99">
-        <v>21</v>
+        <v>6386</v>
       </c>
       <c r="D99">
-        <v>3</v>
+        <v>270</v>
       </c>
       <c r="E99">
-        <v>14.285714285714279</v>
+        <v>4.2279987472596314</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A100">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B100" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C100">
-        <v>118</v>
+        <v>6765</v>
       </c>
       <c r="D100">
-        <v>16</v>
+        <v>262</v>
       </c>
       <c r="E100">
-        <v>13.559322033898299</v>
+        <v>3.8728750923872872</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A101">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="B101" t="s">
         <v>5</v>
       </c>
       <c r="C101">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="D101">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E101">
-        <v>20</v>
+        <v>3.773584905660377</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A102">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="B102" t="s">
         <v>6</v>
       </c>
       <c r="C102">
-        <v>28</v>
+        <v>1965</v>
       </c>
       <c r="D102">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="E102">
-        <v>17.857142857142861</v>
+        <v>3.7659033078880402</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A103">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="B103" t="s">
         <v>7</v>
       </c>
       <c r="C103">
-        <v>26</v>
+        <v>15846</v>
       </c>
       <c r="D103">
-        <v>4</v>
+        <v>593</v>
       </c>
       <c r="E103">
-        <v>15.38461538461539</v>
+        <v>3.7422693424208</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A104">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="B104" t="s">
         <v>5</v>
       </c>
       <c r="C104">
-        <v>4</v>
+        <v>23192</v>
       </c>
       <c r="D104">
-        <v>0</v>
+        <v>843</v>
       </c>
       <c r="E104">
-        <v>0</v>
+        <v>3.6348740945153502</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A105">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="B105" t="s">
         <v>6</v>
       </c>
       <c r="C105">
-        <v>14</v>
+        <v>4019</v>
       </c>
       <c r="D105">
-        <v>4</v>
+        <v>140</v>
       </c>
       <c r="E105">
-        <v>28.571428571428569</v>
+        <v>3.4834535954217469</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A106">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="B106" t="s">
         <v>7</v>
       </c>
       <c r="C106">
-        <v>17</v>
+        <v>32596</v>
       </c>
       <c r="D106">
-        <v>1</v>
+        <v>1118</v>
       </c>
       <c r="E106">
-        <v>5.8823529411764701</v>
+        <v>3.429868695545466</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A107">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B107" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C107">
-        <v>5</v>
+        <v>3854</v>
       </c>
       <c r="D107">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="E107">
-        <v>60</v>
+        <v>2.698495070057084</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A108">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="B108" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C108">
-        <v>13</v>
+        <v>11804</v>
       </c>
       <c r="D108">
-        <v>5</v>
+        <v>290</v>
       </c>
       <c r="E108">
-        <v>38.461538461538467</v>
+        <v>2.456794307014571</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A109">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="B109" t="s">
         <v>7</v>
       </c>
       <c r="C109">
-        <v>18</v>
+        <v>14229</v>
       </c>
       <c r="D109">
-        <v>2</v>
+        <v>308</v>
       </c>
       <c r="E109">
-        <v>11.111111111111111</v>
+        <v>2.1645934359406849</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A110">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="B110" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C110">
-        <v>3</v>
+        <v>7560</v>
       </c>
       <c r="D110">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E110">
-        <v>33.333333333333329</v>
+        <v>2.0238095238095242</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A111">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="B111" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C111">
-        <v>6</v>
+        <v>5985</v>
       </c>
       <c r="D111">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="E111">
-        <v>0</v>
+        <v>1.7878028404344199</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A112">
+        <v>19</v>
+      </c>
+      <c r="B112" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112">
+        <v>2967</v>
+      </c>
+      <c r="D112">
         <v>52</v>
       </c>
-      <c r="B112" t="s">
-        <v>7</v>
-      </c>
-      <c r="C112">
-        <v>20</v>
-      </c>
-      <c r="D112">
-        <v>1</v>
-      </c>
       <c r="E112">
-        <v>5</v>
+        <v>1.7526120660599931</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A113">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B113" t="s">
         <v>5</v>
       </c>
       <c r="C113">
-        <v>1</v>
+        <v>440</v>
       </c>
       <c r="D113">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E113">
-        <v>0</v>
+        <v>1.5909090909090911</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A114">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B114" t="s">
         <v>7</v>
       </c>
       <c r="C114">
-        <v>16</v>
+        <v>847</v>
       </c>
       <c r="D114">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E114">
-        <v>31.25</v>
+        <v>1.1806375442739081</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A115">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="B115" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C115">
-        <v>3</v>
+        <v>551</v>
       </c>
       <c r="D115">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E115">
-        <v>0</v>
+        <v>0.72595281306715065</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A116">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="B116" t="s">
         <v>6</v>
       </c>
       <c r="C116">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -2395,30 +2398,30 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A117">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B117" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C117">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D117">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E117">
-        <v>15.38461538461539</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A118">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B118" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C118">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -2429,47 +2432,47 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A119">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B119" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C119">
         <v>1</v>
       </c>
       <c r="D119">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E119">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A120">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B120" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C120">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D120">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E120">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A121">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B121" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C121">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D121">
         <v>0</v>
@@ -2480,13 +2483,13 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A122">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B122" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C122">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D122">
         <v>0</v>
@@ -2497,36 +2500,36 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A123">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B123" t="s">
         <v>5</v>
       </c>
       <c r="C123">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D123">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E123">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A124">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B124" t="s">
         <v>7</v>
       </c>
       <c r="C124">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D124">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E124">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.45">
@@ -2547,6 +2550,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E125">
+    <sortCondition descending="1" ref="E2:E125"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2555,7 +2561,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -2584,53 +2592,53 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2">
-        <v>334</v>
+        <v>58</v>
       </c>
       <c r="D2">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="E2">
-        <v>18.26347305389222</v>
+        <v>27.586206896551719</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3">
-        <v>456</v>
+        <v>115</v>
       </c>
       <c r="D3">
-        <v>94</v>
+        <v>24</v>
       </c>
       <c r="E3">
-        <v>20.614035087719301</v>
+        <v>20.869565217391301</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>335</v>
+        <v>456</v>
       </c>
       <c r="D4">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="E4">
-        <v>20.597014925373131</v>
+        <v>20.614035087719301</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -2638,33 +2646,33 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>526</v>
+        <v>335</v>
       </c>
       <c r="D5">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="E5">
-        <v>20.342205323193919</v>
+        <v>20.597014925373131</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6">
-        <v>751</v>
+        <v>526</v>
       </c>
       <c r="D6">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="E6">
-        <v>18.90812250332889</v>
+        <v>20.342205323193919</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -2686,36 +2694,36 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8">
-        <v>115</v>
+        <v>751</v>
       </c>
       <c r="D8">
-        <v>24</v>
+        <v>142</v>
       </c>
       <c r="E8">
-        <v>20.869565217391301</v>
+        <v>18.90812250332889</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>131</v>
+        <v>334</v>
       </c>
       <c r="D9">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="E9">
-        <v>16.03053435114504</v>
+        <v>18.26347305389222</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
@@ -2723,19 +2731,22 @@
         <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10">
-        <v>58</v>
+        <v>131</v>
       </c>
       <c r="D10">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E10">
-        <v>27.586206896551719</v>
+        <v>16.03053435114504</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E10">
+    <sortCondition descending="1" ref="E2:E10"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>